<commit_message>
arquivos da detecção das EPI's finalizados.
</commit_message>
<xml_diff>
--- a/data/Bruno Nunes Teixeira.xlsx
+++ b/data/Bruno Nunes Teixeira.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,66 @@
           <t>08/09/2022</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>14/9/2022</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>15/9/2022</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>19/9/2022</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>20/9/2022</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>21/9/2022</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>22/9/2022</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>23/9/2022</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>24/9/2022</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>26/9/2022</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>27/9/2022</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>28/9/2022</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>29/9/2022</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -469,6 +529,66 @@
           <t>sim</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -489,6 +609,66 @@
           <t>sim</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -509,6 +689,66 @@
           <t>-</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -529,6 +769,66 @@
           <t>sim</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -549,6 +849,66 @@
           <t>sim</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -565,6 +925,66 @@
         </is>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>sim</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>não</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
         <is>
           <t>-</t>
         </is>

</xml_diff>